<commit_message>
eerste toevoegingen van algemene model inclusief visualisatie
</commit_message>
<xml_diff>
--- a/nodes_loc.xlsx
+++ b/nodes_loc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9169fa5a3c35e09c/Bureaublad/Jilles/AE/MSc/AE4441_Operations_Optimization/VRP_assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC104869D99874AA5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5DC46F5-A0EB-4F96-9CC9-BD961B7C9AD1}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_F25DC773A252ABDACC104869D99874AA5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D295A73F-0F46-40D8-B52A-268E77A9D75D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loc" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
-  <si>
-    <t>central</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>ac_1</t>
-  </si>
-  <si>
-    <t>ac_2</t>
-  </si>
-  <si>
-    <t>ac_3</t>
-  </si>
-  <si>
-    <t>ac_4</t>
-  </si>
-  <si>
-    <t>ac_5</t>
-  </si>
-  <si>
-    <t>ac_6</t>
   </si>
 </sst>
 </file>
@@ -386,96 +365,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
         <v>-1</v>
       </c>
     </row>
@@ -487,265 +445,221 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A608E6D-4040-41DB-BA7C-18DF6A15DFD9}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>SQRT((loc!A2-loc!$A$2)^2+(loc!B2-loc!$B$2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>SQRT((loc!$A2-loc!$A$3)^2+(loc!$B2-loc!$B$3)^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="C1">
+        <f>SQRT((loc!$A2-loc!$A$4)^2+(loc!$B2-loc!$B$4)^2)</f>
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f>SQRT((loc!$A2-loc!$A$5)^2+(loc!$B2-loc!$B$5)^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="E1">
+        <f>SQRT((loc!$A2-loc!$A$6)^2+(loc!$B2-loc!$B$6)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="F1">
+        <f>SQRT((loc!$A2-loc!$A$7)^2+(loc!$B2-loc!$B$7)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <f>SQRT((loc!$A2-loc!$A$8)^2+(loc!$B2-loc!$B$8)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>SQRT((loc!A3-loc!$A$2)^2+(loc!B3-loc!$B$2)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="B2">
-        <f>SQRT((loc!B2-loc!$B$2)^2+(loc!C2-loc!$C$2)^2)</f>
+        <f>SQRT((loc!$A3-loc!$A$3)^2+(loc!$B3-loc!$B$3)^2)</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SQRT((loc!$B2-loc!$B$3)^2+(loc!$C2-loc!$C$3)^2)</f>
-        <v>1.4142135623730951</v>
+        <f>SQRT((loc!$A3-loc!$A$4)^2+(loc!$B3-loc!$B$4)^2)</f>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>SQRT((loc!$B2-loc!$B$4)^2+(loc!$C2-loc!$C$4)^2)</f>
-        <v>1</v>
+        <f>SQRT((loc!$A3-loc!$A$5)^2+(loc!$B3-loc!$B$5)^2)</f>
+        <v>2</v>
       </c>
       <c r="E2">
-        <f>SQRT((loc!$B2-loc!$B$5)^2+(loc!$C2-loc!$C$5)^2)</f>
-        <v>1.4142135623730951</v>
+        <f>SQRT((loc!$A3-loc!$A$6)^2+(loc!$B3-loc!$B$6)^2)</f>
+        <v>1</v>
       </c>
       <c r="F2">
-        <f>SQRT((loc!$B2-loc!$B$6)^2+(loc!$C2-loc!$C$6)^2)</f>
-        <v>2.2360679774997898</v>
+        <f>SQRT((loc!$A3-loc!$A$7)^2+(loc!$B3-loc!$B$7)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="G2">
-        <f>SQRT((loc!$B2-loc!$B$7)^2+(loc!$C2-loc!$C$7)^2)</f>
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <f>SQRT((loc!$B2-loc!$B$8)^2+(loc!$C2-loc!$C$8)^2)</f>
-        <v>2.2360679774997898</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+        <f>SQRT((loc!$A3-loc!$A$8)^2+(loc!$B3-loc!$B$8)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SQRT((loc!A4-loc!$A$2)^2+(loc!B4-loc!$B$2)^2)</f>
+        <v>1</v>
       </c>
       <c r="B3">
-        <f>SQRT((loc!B3-loc!$B$2)^2+(loc!C3-loc!$C$2)^2)</f>
-        <v>1.4142135623730951</v>
+        <f>SQRT((loc!$A4-loc!$A$3)^2+(loc!$B4-loc!$B$3)^2)</f>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>SQRT((loc!$B3-loc!$B$3)^2+(loc!$C3-loc!$C$3)^2)</f>
+        <f>SQRT((loc!$A4-loc!$A$4)^2+(loc!$B4-loc!$B$4)^2)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>SQRT((loc!$B3-loc!$B$4)^2+(loc!$C3-loc!$C$4)^2)</f>
+        <f>SQRT((loc!$A4-loc!$A$5)^2+(loc!$B4-loc!$B$5)^2)</f>
         <v>1</v>
       </c>
       <c r="E3">
-        <f>SQRT((loc!$B3-loc!$B$5)^2+(loc!$C3-loc!$C$5)^2)</f>
-        <v>2</v>
+        <f>SQRT((loc!$A4-loc!$A$6)^2+(loc!$B4-loc!$B$6)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="F3">
-        <f>SQRT((loc!$B3-loc!$B$6)^2+(loc!$C3-loc!$C$6)^2)</f>
+        <f>SQRT((loc!$A4-loc!$A$7)^2+(loc!$B4-loc!$B$7)^2)</f>
         <v>1</v>
       </c>
       <c r="G3">
-        <f>SQRT((loc!$B3-loc!$B$7)^2+(loc!$C3-loc!$C$7)^2)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="H3">
-        <f>SQRT((loc!$B3-loc!$B$8)^2+(loc!$C3-loc!$C$8)^2)</f>
-        <v>2.2360679774997898</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
+        <f>SQRT((loc!$A4-loc!$A$8)^2+(loc!$B4-loc!$B$8)^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>SQRT((loc!A5-loc!$A$2)^2+(loc!B5-loc!$B$2)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="B4">
-        <f>SQRT((loc!B4-loc!$B$2)^2+(loc!C4-loc!$C$2)^2)</f>
-        <v>1</v>
+        <f>SQRT((loc!$A5-loc!$A$3)^2+(loc!$B5-loc!$B$3)^2)</f>
+        <v>2</v>
       </c>
       <c r="C4">
-        <f>SQRT((loc!$B4-loc!$B$3)^2+(loc!$C4-loc!$C$3)^2)</f>
+        <f>SQRT((loc!$A5-loc!$A$4)^2+(loc!$B5-loc!$B$4)^2)</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f>SQRT((loc!$B4-loc!$B$4)^2+(loc!$C4-loc!$C$4)^2)</f>
+        <f>SQRT((loc!$A5-loc!$A$5)^2+(loc!$B5-loc!$B$5)^2)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SQRT((loc!$B4-loc!$B$5)^2+(loc!$C4-loc!$C$5)^2)</f>
-        <v>1</v>
+        <f>SQRT((loc!$A5-loc!$A$6)^2+(loc!$B5-loc!$B$6)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="F4">
-        <f>SQRT((loc!$B4-loc!$B$6)^2+(loc!$C4-loc!$C$6)^2)</f>
+        <f>SQRT((loc!$A5-loc!$A$7)^2+(loc!$B5-loc!$B$7)^2)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="G4">
-        <f>SQRT((loc!$B4-loc!$B$7)^2+(loc!$C4-loc!$C$7)^2)</f>
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <f>SQRT((loc!$B4-loc!$B$8)^2+(loc!$C4-loc!$C$8)^2)</f>
-        <v>1.4142135623730951</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
+        <f>SQRT((loc!$A5-loc!$A$8)^2+(loc!$B5-loc!$B$8)^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>SQRT((loc!A6-loc!$A$2)^2+(loc!B6-loc!$B$2)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="B5">
-        <f>SQRT((loc!B5-loc!$B$2)^2+(loc!C5-loc!$C$2)^2)</f>
-        <v>1.4142135623730951</v>
+        <f>SQRT((loc!$A6-loc!$A$3)^2+(loc!$B6-loc!$B$3)^2)</f>
+        <v>1</v>
       </c>
       <c r="C5">
-        <f>SQRT((loc!$B5-loc!$B$3)^2+(loc!$C5-loc!$C$3)^2)</f>
-        <v>2</v>
+        <f>SQRT((loc!$A6-loc!$A$4)^2+(loc!$B6-loc!$B$4)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="D5">
-        <f>SQRT((loc!$B5-loc!$B$4)^2+(loc!$C5-loc!$C$4)^2)</f>
-        <v>1</v>
+        <f>SQRT((loc!$A6-loc!$A$5)^2+(loc!$B6-loc!$B$5)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="E5">
-        <f>SQRT((loc!$B5-loc!$B$5)^2+(loc!$C5-loc!$C$5)^2)</f>
+        <f>SQRT((loc!$A6-loc!$A$6)^2+(loc!$B6-loc!$B$6)^2)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>SQRT((loc!$B5-loc!$B$6)^2+(loc!$C5-loc!$C$6)^2)</f>
-        <v>2.2360679774997898</v>
+        <f>SQRT((loc!$A6-loc!$A$7)^2+(loc!$B6-loc!$B$7)^2)</f>
+        <v>1</v>
       </c>
       <c r="G5">
-        <f>SQRT((loc!$B5-loc!$B$7)^2+(loc!$C5-loc!$C$7)^2)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="H5">
-        <f>SQRT((loc!$B5-loc!$B$8)^2+(loc!$C5-loc!$C$8)^2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
+        <f>SQRT((loc!$A6-loc!$A$8)^2+(loc!$B6-loc!$B$8)^2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>SQRT((loc!A7-loc!$A$2)^2+(loc!B7-loc!$B$2)^2)</f>
+        <v>2</v>
       </c>
       <c r="B6">
-        <f>SQRT((loc!B6-loc!$B$2)^2+(loc!C6-loc!$C$2)^2)</f>
-        <v>2.2360679774997898</v>
+        <f>SQRT((loc!$A7-loc!$A$3)^2+(loc!$B7-loc!$B$3)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="C6">
-        <f>SQRT((loc!$B6-loc!$B$3)^2+(loc!$C6-loc!$C$3)^2)</f>
+        <f>SQRT((loc!$A7-loc!$A$4)^2+(loc!$B7-loc!$B$4)^2)</f>
         <v>1</v>
       </c>
       <c r="D6">
-        <f>SQRT((loc!$B6-loc!$B$4)^2+(loc!$C6-loc!$C$4)^2)</f>
+        <f>SQRT((loc!$A7-loc!$A$5)^2+(loc!$B7-loc!$B$5)^2)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="E6">
-        <f>SQRT((loc!$B6-loc!$B$5)^2+(loc!$C6-loc!$C$5)^2)</f>
-        <v>2.2360679774997898</v>
+        <f>SQRT((loc!$A7-loc!$A$6)^2+(loc!$B7-loc!$B$6)^2)</f>
+        <v>1</v>
       </c>
       <c r="F6">
-        <f>SQRT((loc!$B6-loc!$B$6)^2+(loc!$C6-loc!$C$6)^2)</f>
+        <f>SQRT((loc!$A7-loc!$A$7)^2+(loc!$B7-loc!$B$7)^2)</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SQRT((loc!$B6-loc!$B$7)^2+(loc!$C6-loc!$C$7)^2)</f>
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <f>SQRT((loc!$B6-loc!$B$8)^2+(loc!$C6-loc!$C$8)^2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
+        <f>SQRT((loc!$A7-loc!$A$8)^2+(loc!$B7-loc!$B$8)^2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>SQRT((loc!A8-loc!$A$2)^2+(loc!B8-loc!$B$2)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="B7">
-        <f>SQRT((loc!B7-loc!$B$2)^2+(loc!C7-loc!$C$2)^2)</f>
-        <v>2</v>
+        <f>SQRT((loc!$A8-loc!$A$3)^2+(loc!$B8-loc!$B$3)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="C7">
-        <f>SQRT((loc!$B7-loc!$B$3)^2+(loc!$C7-loc!$C$3)^2)</f>
+        <f>SQRT((loc!$A8-loc!$A$4)^2+(loc!$B8-loc!$B$4)^2)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="D7">
-        <f>SQRT((loc!$B7-loc!$B$4)^2+(loc!$C7-loc!$C$4)^2)</f>
+        <f>SQRT((loc!$A8-loc!$A$5)^2+(loc!$B8-loc!$B$5)^2)</f>
         <v>1</v>
       </c>
       <c r="E7">
-        <f>SQRT((loc!$B7-loc!$B$5)^2+(loc!$C7-loc!$C$5)^2)</f>
-        <v>1.4142135623730951</v>
+        <f>SQRT((loc!$A8-loc!$A$6)^2+(loc!$B8-loc!$B$6)^2)</f>
+        <v>2</v>
       </c>
       <c r="F7">
-        <f>SQRT((loc!$B7-loc!$B$6)^2+(loc!$C7-loc!$C$6)^2)</f>
+        <f>SQRT((loc!$A8-loc!$A$7)^2+(loc!$B8-loc!$B$7)^2)</f>
         <v>1</v>
       </c>
       <c r="G7">
-        <f>SQRT((loc!$B7-loc!$B$7)^2+(loc!$C7-loc!$C$7)^2)</f>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>SQRT((loc!$B7-loc!$B$8)^2+(loc!$C7-loc!$C$8)^2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <f>SQRT((loc!B8-loc!$B$2)^2+(loc!C8-loc!$C$2)^2)</f>
-        <v>2.2360679774997898</v>
-      </c>
-      <c r="C8">
-        <f>SQRT((loc!$B8-loc!$B$3)^2+(loc!$C8-loc!$C$3)^2)</f>
-        <v>2.2360679774997898</v>
-      </c>
-      <c r="D8">
-        <f>SQRT((loc!$B8-loc!$B$4)^2+(loc!$C8-loc!$C$4)^2)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="E8">
-        <f>SQRT((loc!$B8-loc!$B$5)^2+(loc!$C8-loc!$C$5)^2)</f>
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f>SQRT((loc!$B8-loc!$B$6)^2+(loc!$C8-loc!$C$6)^2)</f>
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <f>SQRT((loc!$B8-loc!$B$7)^2+(loc!$C8-loc!$C$7)^2)</f>
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <f>SQRT((loc!$B8-loc!$B$8)^2+(loc!$C8-loc!$C$8)^2)</f>
+        <f>SQRT((loc!$A8-loc!$A$8)^2+(loc!$B8-loc!$B$8)^2)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>